<commit_message>
Small typos in Second Order Stations pressure data fixed
</commit_message>
<xml_diff>
--- a/second-order/1875/August1875.xlsx
+++ b/second-order/1875/August1875.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\expnaspre\library_archive$\ARCHIVE\Data\Second Order Books - KEYING\1875\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/weather-rescue/second-order/1875/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5797" documentId="13_ncr:1_{955945B9-7D0A-4A40-B2A5-8518FA235476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66C06E96-5955-4524-B36B-BA669FE8A0BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104EB0A9-F242-5445-87A6-7A2CF7E655C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="8" xr2:uid="{F301734F-2AF4-4BAC-817B-B629B6303572}"/>
+    <workbookView xWindow="2780" yWindow="2620" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{F301734F-2AF4-4BAC-817B-B629B6303572}"/>
   </bookViews>
   <sheets>
     <sheet name="Hawes" sheetId="1" r:id="rId1"/>
@@ -250,7 +250,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,6 +563,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,15 +588,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -608,9 +608,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -648,7 +648,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -754,7 +754,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -896,7 +896,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -908,60 +908,60 @@
   <dimension ref="A2:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="C27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E4" sqref="E4"/>
       <selection pane="bottomLeft" activeCell="U36" sqref="U36"/>
-      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>19</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>19</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>19</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>19</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>19</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>19</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>19</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -3120,59 +3120,59 @@
   <dimension ref="A2:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="I26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>38</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>38</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>0.309</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="D12" s="1">
         <v>9</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="33">
         <v>29.803000000000001</v>
       </c>
       <c r="F12" s="6">
@@ -3822,7 +3822,7 @@
         <v>0.255</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>1.5029999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>38</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>38</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>38</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>38</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>0.109</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>38</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>0.33200000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -5331,59 +5331,59 @@
   <dimension ref="A2:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="E27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>46</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>46</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>46</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>46</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>0.16400000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -6566,7 +6566,7 @@
       <c r="D21" s="1">
         <v>18</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="34">
         <v>30</v>
       </c>
       <c r="F21" s="6">
@@ -6618,7 +6618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
@@ -6748,7 +6748,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>46</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>46</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>46</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>46</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>46</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>46</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
@@ -7268,7 +7268,7 @@
         <v>0.218</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>46</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>46</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>46</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -7542,59 +7542,59 @@
   <dimension ref="A2:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="I25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -7659,7 +7659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>49</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>49</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>49</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
@@ -8439,7 +8439,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
@@ -8699,7 +8699,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>49</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
@@ -8894,7 +8894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>49</v>
       </c>
@@ -8959,7 +8959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>49</v>
       </c>
@@ -9089,7 +9089,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
@@ -9154,7 +9154,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>49</v>
       </c>
@@ -9219,7 +9219,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>49</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>49</v>
       </c>
@@ -9349,7 +9349,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>49</v>
       </c>
@@ -9414,7 +9414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>49</v>
       </c>
@@ -9479,7 +9479,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>49</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>49</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>49</v>
       </c>
@@ -9674,7 +9674,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -9753,59 +9753,59 @@
   <dimension ref="A2:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="I30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -9870,7 +9870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>50</v>
       </c>
@@ -9935,7 +9935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>50</v>
       </c>
@@ -10000,7 +10000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>50</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>50</v>
       </c>
@@ -10130,7 +10130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -10195,7 +10195,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
@@ -10260,7 +10260,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
@@ -10325,7 +10325,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>50</v>
       </c>
@@ -10390,7 +10390,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -10455,7 +10455,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -10520,7 +10520,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>50</v>
       </c>
@@ -10585,7 +10585,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
@@ -10715,7 +10715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -10780,7 +10780,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -10845,7 +10845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>50</v>
       </c>
@@ -10910,7 +10910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>50</v>
       </c>
@@ -10975,7 +10975,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -11040,7 +11040,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>50</v>
       </c>
@@ -11105,7 +11105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
@@ -11170,7 +11170,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>50</v>
       </c>
@@ -11235,7 +11235,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>50</v>
       </c>
@@ -11300,7 +11300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>50</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
@@ -11495,7 +11495,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>50</v>
       </c>
@@ -11560,7 +11560,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
@@ -11625,7 +11625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>50</v>
       </c>
@@ -11690,7 +11690,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
@@ -11755,7 +11755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>50</v>
       </c>
@@ -11820,7 +11820,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>50</v>
       </c>
@@ -11885,7 +11885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -11964,59 +11964,59 @@
   <dimension ref="A2:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="I25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -12081,7 +12081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
@@ -12146,7 +12146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -12211,7 +12211,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>58</v>
       </c>
@@ -12276,7 +12276,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>58</v>
       </c>
@@ -12341,7 +12341,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
@@ -12406,7 +12406,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>58</v>
       </c>
@@ -12471,7 +12471,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
@@ -12536,7 +12536,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>58</v>
       </c>
@@ -12601,7 +12601,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>58</v>
       </c>
@@ -12666,7 +12666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>58</v>
       </c>
@@ -12731,7 +12731,7 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>58</v>
       </c>
@@ -12796,7 +12796,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>58</v>
       </c>
@@ -12861,7 +12861,7 @@
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>58</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>58</v>
       </c>
@@ -12991,7 +12991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -13056,7 +13056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
@@ -13186,7 +13186,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>58</v>
       </c>
@@ -13251,7 +13251,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>58</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>0.41499999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>58</v>
       </c>
@@ -13381,7 +13381,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>58</v>
       </c>
@@ -13446,7 +13446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>58</v>
       </c>
@@ -13511,7 +13511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
@@ -13576,7 +13576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>58</v>
       </c>
@@ -13641,7 +13641,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
@@ -13706,7 +13706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>58</v>
       </c>
@@ -13771,7 +13771,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>58</v>
       </c>
@@ -13836,7 +13836,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>58</v>
       </c>
@@ -13901,7 +13901,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>58</v>
       </c>
@@ -13966,7 +13966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>58</v>
       </c>
@@ -14031,7 +14031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>58</v>
       </c>
@@ -14096,7 +14096,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -14175,59 +14175,59 @@
   <dimension ref="A2:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="N26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -14292,7 +14292,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>60</v>
       </c>
@@ -14357,7 +14357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
@@ -14422,7 +14422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>60</v>
       </c>
@@ -14487,7 +14487,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>60</v>
       </c>
@@ -14552,7 +14552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>60</v>
       </c>
@@ -14617,7 +14617,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
@@ -14682,7 +14682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>60</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>60</v>
       </c>
@@ -14812,7 +14812,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>60</v>
       </c>
@@ -14877,7 +14877,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>60</v>
       </c>
@@ -14942,7 +14942,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>60</v>
       </c>
@@ -14955,7 +14955,7 @@
       <c r="D14" s="1">
         <v>11</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="34">
         <v>30</v>
       </c>
       <c r="F14" s="6">
@@ -15007,7 +15007,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>60</v>
       </c>
@@ -15072,7 +15072,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>60</v>
       </c>
@@ -15137,7 +15137,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>60</v>
       </c>
@@ -15202,7 +15202,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>60</v>
       </c>
@@ -15267,7 +15267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>60</v>
       </c>
@@ -15332,7 +15332,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>60</v>
       </c>
@@ -15397,7 +15397,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>60</v>
       </c>
@@ -15462,7 +15462,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>60</v>
       </c>
@@ -15527,7 +15527,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>60</v>
       </c>
@@ -15592,7 +15592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>60</v>
       </c>
@@ -15657,7 +15657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>60</v>
       </c>
@@ -15722,7 +15722,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
@@ -15787,7 +15787,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>60</v>
       </c>
@@ -15852,7 +15852,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
@@ -15917,7 +15917,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>60</v>
       </c>
@@ -15982,7 +15982,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>60</v>
       </c>
@@ -16047,7 +16047,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>60</v>
       </c>
@@ -16112,7 +16112,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>60</v>
       </c>
@@ -16177,7 +16177,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>60</v>
       </c>
@@ -16242,7 +16242,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>60</v>
       </c>
@@ -16307,7 +16307,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -16385,60 +16385,60 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:XFD36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="B26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -16503,7 +16503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>61</v>
       </c>
@@ -16568,7 +16568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
@@ -16633,7 +16633,7 @@
         <v>0.29399999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>61</v>
       </c>
@@ -16698,7 +16698,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>61</v>
       </c>
@@ -16763,7 +16763,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>61</v>
       </c>
@@ -16828,7 +16828,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>61</v>
       </c>
@@ -16893,7 +16893,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>61</v>
       </c>
@@ -16958,7 +16958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -16972,7 +16972,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="5">
-        <v>31.030999999999999</v>
+        <v>30.030999999999999</v>
       </c>
       <c r="F11" s="6">
         <v>29.931000000000001</v>
@@ -17023,7 +17023,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
@@ -17088,7 +17088,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>61</v>
       </c>
@@ -17153,7 +17153,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
@@ -17218,7 +17218,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>61</v>
       </c>
@@ -17283,7 +17283,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
@@ -17348,7 +17348,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>61</v>
       </c>
@@ -17413,7 +17413,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>61</v>
       </c>
@@ -17478,7 +17478,7 @@
         <v>0.38300000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>61</v>
       </c>
@@ -17543,7 +17543,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>61</v>
       </c>
@@ -17608,7 +17608,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>61</v>
       </c>
@@ -17673,7 +17673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>61</v>
       </c>
@@ -17738,7 +17738,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>61</v>
       </c>
@@ -17803,7 +17803,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>61</v>
       </c>
@@ -17868,7 +17868,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>61</v>
       </c>
@@ -17933,7 +17933,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>61</v>
       </c>
@@ -17998,7 +17998,7 @@
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>61</v>
       </c>
@@ -18063,7 +18063,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>61</v>
       </c>
@@ -18128,7 +18128,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
@@ -18193,7 +18193,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>61</v>
       </c>
@@ -18258,7 +18258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>61</v>
       </c>
@@ -18323,7 +18323,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>61</v>
       </c>
@@ -18388,7 +18388,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21 16384:16384">
+    <row r="33" spans="1:21 16384:16384" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>61</v>
       </c>
@@ -18453,7 +18453,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:21 16384:16384">
+    <row r="34" spans="1:21 16384:16384" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>61</v>
       </c>
@@ -18518,7 +18518,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:21 16384:16384">
+    <row r="35" spans="1:21 16384:16384" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -18577,7 +18577,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="36" spans="1:21 16384:16384">
+    <row r="36" spans="1:21 16384:16384" x14ac:dyDescent="0.2">
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
@@ -18614,60 +18614,60 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="8.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="8.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="2" customFormat="1">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="33" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="33" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="37" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="33" t="s">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="34"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1">
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -18732,7 +18732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>63</v>
       </c>
@@ -18797,7 +18797,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
@@ -18862,7 +18862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>63</v>
       </c>
@@ -18927,7 +18927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>63</v>
       </c>
@@ -18992,7 +18992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>63</v>
       </c>
@@ -19057,7 +19057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>63</v>
       </c>
@@ -19122,7 +19122,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>63</v>
       </c>
@@ -19187,7 +19187,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>63</v>
       </c>
@@ -19252,7 +19252,7 @@
         <v>0.33100000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>63</v>
       </c>
@@ -19317,7 +19317,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>63</v>
       </c>
@@ -19382,7 +19382,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>63</v>
       </c>
@@ -19447,7 +19447,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>63</v>
       </c>
@@ -19512,7 +19512,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
@@ -19577,7 +19577,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>63</v>
       </c>
@@ -19642,7 +19642,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>63</v>
       </c>
@@ -19707,7 +19707,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>63</v>
       </c>
@@ -19772,7 +19772,7 @@
         <v>1.046</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>63</v>
       </c>
@@ -19837,7 +19837,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>63</v>
       </c>
@@ -19902,7 +19902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>63</v>
       </c>
@@ -19967,7 +19967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
@@ -20032,7 +20032,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>63</v>
       </c>
@@ -20097,7 +20097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>63</v>
       </c>
@@ -20162,7 +20162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>63</v>
       </c>
@@ -20227,7 +20227,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
@@ -20292,7 +20292,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>63</v>
       </c>
@@ -20357,7 +20357,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>63</v>
       </c>
@@ -20422,7 +20422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>63</v>
       </c>
@@ -20487,7 +20487,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>63</v>
       </c>
@@ -20552,7 +20552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>63</v>
       </c>
@@ -20592,7 +20592,7 @@
       <c r="M32" s="1">
         <v>85</v>
       </c>
-      <c r="N32" s="41">
+      <c r="N32" s="35">
         <v>85</v>
       </c>
       <c r="O32" s="22" t="s">
@@ -20617,7 +20617,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>63</v>
       </c>
@@ -20682,7 +20682,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>63</v>
       </c>
@@ -20747,7 +20747,7 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -20821,35 +20821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Preview xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Preview>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">H7Q62YT2XCZT-908671883-27387</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">
-      <Url>https://metoffice.sharepoint.com/sites/metofficelibraryarchiveteam/_layouts/15/DocIdRedir.aspx?ID=H7Q62YT2XCZT-908671883-27387</Url>
-      <Description>H7Q62YT2XCZT-908671883-27387</Description>
-    </_dlc_DocIdUrl>
-    <_Flow_SignoffStatus xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xsi:nil="true"/>
-    <TaxCatchAll xmlns="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -20897,6 +20868,35 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Preview xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Preview>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">H7Q62YT2XCZT-908671883-27387</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">
+      <Url>https://metoffice.sharepoint.com/sites/metofficelibraryarchiveteam/_layouts/15/DocIdRedir.aspx?ID=H7Q62YT2XCZT-908671883-27387</Url>
+      <Description>H7Q62YT2XCZT-908671883-27387</Description>
+    </_dlc_DocIdUrl>
+    <_Flow_SignoffStatus xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xsi:nil="true"/>
+    <TaxCatchAll xmlns="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21201,17 +21201,51 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7739F49B-73A7-4E5F-A4ED-21ACA989FEE3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E24A8245-7510-4D20-AA33-E706D7D890BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{244BB8A5-B09D-4473-BEF9-DAA9B4742265}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{244BB8A5-B09D-4473-BEF9-DAA9B4742265}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="09baef80-0d7a-4cab-b988-bb3d9fc0663b"/>
+    <ds:schemaRef ds:uri="502a79df-4f52-4757-ac2f-753e065f4c93"/>
+    <ds:schemaRef ds:uri="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E24A8245-7510-4D20-AA33-E706D7D890BA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7739F49B-73A7-4E5F-A4ED-21ACA989FEE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AA1954-9B42-4079-816F-0DAD6B1F1218}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AA1954-9B42-4079-816F-0DAD6B1F1218}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="09baef80-0d7a-4cab-b988-bb3d9fc0663b"/>
+    <ds:schemaRef ds:uri="502a79df-4f52-4757-ac2f-753e065f4c93"/>
+    <ds:schemaRef ds:uri="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>